<commit_message>
excel sheets data & reports
</commit_message>
<xml_diff>
--- a/NopCommerce/Test_Reports/TC_AddToCartTest_Report.xlsx
+++ b/NopCommerce/Test_Reports/TC_AddToCartTest_Report.xlsx
@@ -1,56 +1,137 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT_Projects\NopCommerce\Test_Reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result (After Execution)</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Comments (Optional)</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>Search and pick 'HTC One Mini Blue' (without clicking the item card)</t>
+  </si>
+  <si>
+    <t>Item added successfully</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>Pick 'Build your own computer'  from Home page(by clicking the item card)</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>item quantity added successfully</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>Check cart updates (Following TC_03 Steps)</t>
+  </si>
+  <si>
+    <t>Items added matches the cart content (Following TC_03 steps)</t>
+  </si>
+  <si>
+    <t>Follow up cart successfully checked</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>Remove item from cart (0 items in cart) (Following TC_04)</t>
+  </si>
+  <si>
+    <t>item removal successful</t>
+  </si>
+  <si>
+    <t>Cart becomes empty after removing the item</t>
+  </si>
+  <si>
+    <t>Notification "item added successfully"</t>
+  </si>
+  <si>
+    <t>Add item by clicking on add to cart twice</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="0"/>
-      <sz val="13"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color theme="0"/>
-      <sz val="13"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Inherit"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="13"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -63,7 +144,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.3999755851924192"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -96,98 +177,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -477,201 +499,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col width="15.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="41.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="38" customWidth="1" min="3" max="3"/>
-    <col width="36.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="13.140625" customWidth="1" min="5" max="5"/>
-    <col width="98.140625" customWidth="1" min="6" max="6"/>
+    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="4" max="4" width="36.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" customWidth="1"/>
+    <col min="6" max="6" width="98.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Test Case ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Expected Result</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Actual Result (After Execution)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Pass/Fail</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Comments (Optional)</t>
-        </is>
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>TC_01</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Search and pick 'HTC One Mini Blue' (without clicking the item card)</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Notification item added successfully</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="inlineStr">
-        <is>
-          <t>Notification item added successfully</t>
-        </is>
-      </c>
-      <c r="E2" s="6" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="F2" s="6" t="n"/>
+    <row r="2" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
-    <row r="3" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>TC_02</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Pick 'Build your own computer'  from Home page(by clicking the item card)</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>Notification item added successfully</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>Notification item added successfully</t>
-        </is>
-      </c>
-      <c r="E3" s="6" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="F3" s="6" t="n"/>
+    <row r="3" spans="1:6" ht="33.75" thickBot="1">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6"/>
     </row>
-    <row r="4" ht="50.25" customHeight="1" thickBot="1">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>TC_03</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Multiple clicks on add to cart for an amount other than 1</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>Notification items added successfully</t>
-        </is>
-      </c>
-      <c r="D4" s="6" t="inlineStr">
-        <is>
-          <t>item quantity added successfully</t>
-        </is>
-      </c>
-      <c r="E4" s="6" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="F4" s="6" t="n"/>
+    <row r="4" spans="1:6" ht="50.25" customHeight="1" thickBot="1">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6"/>
     </row>
-    <row r="5" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>TC_04</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Check cart updates (Following TC_03 Steps)</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>Items added matches the cart content (Following TC_03 steps)</t>
-        </is>
-      </c>
-      <c r="D5" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Follow up cart successfully checked </t>
-        </is>
-      </c>
-      <c r="E5" s="6" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="F5" s="6" t="n"/>
+    <row r="5" spans="1:6" ht="37.5" customHeight="1" thickBot="1">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6"/>
     </row>
-    <row r="6" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>TC_05</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Remove item from cart (0 items in cart)</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>Cart becomes empty after adding then removing one item</t>
-        </is>
-      </c>
-      <c r="D6" s="6" t="inlineStr">
-        <is>
-          <t>item removal successful</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="F6" s="6" t="n"/>
+    <row r="6" spans="1:6" ht="37.5" customHeight="1" thickBot="1">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="6"/>
     </row>
-    <row r="15">
-      <c r="C15" s="5" t="n"/>
+    <row r="15" spans="1:6">
+      <c r="C15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>